<commit_message>
a little touch ups :sparkles:
</commit_message>
<xml_diff>
--- a/color/comparison_color.xlsx
+++ b/color/comparison_color.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5FCF32-3814-3D49-941A-613370471A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{8DDA7121-79A4-441C-B316-0237A835ED06}"/>
+    <workbookView xWindow="6660" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{8DDA7121-79A4-441C-B316-0237A835ED06}"/>
   </bookViews>
   <sheets>
     <sheet name="RGB" sheetId="1" r:id="rId1"/>
@@ -5658,7 +5658,7 @@
   <dimension ref="A1:L123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B123"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>